<commit_message>
First draft of registration screens and for user research
</commit_message>
<xml_diff>
--- a/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
+++ b/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
@@ -5,20 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63ef8ac642a543be/MyCo/Clients/SFA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63ef8ac642a543be/MyCo/Clients/SFA/Projects/tl-results-prototype/app/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C3B593D-916B-4547-9767-202229F893A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" firstSheet="2" activeTab="3" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" tabRatio="659" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction" sheetId="6" r:id="rId1"/>
-    <sheet name="Add and edit registrations" sheetId="3" r:id="rId2"/>
-    <sheet name="Technical requirements" sheetId="2" r:id="rId3"/>
-    <sheet name="File data items" sheetId="1" r:id="rId4"/>
-    <sheet name="Core and specialism codes" sheetId="4" r:id="rId5"/>
-    <sheet name="Example CSV file" sheetId="5" r:id="rId6"/>
+    <sheet name="How to use this guide" sheetId="6" r:id="rId1"/>
+    <sheet name="File data items and format" sheetId="1" r:id="rId2"/>
+    <sheet name="Core and specialism codes" sheetId="4" r:id="rId3"/>
+    <sheet name="Example CSV file" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Data item</t>
   </si>
@@ -65,42 +63,24 @@
     <t>Unique Learner Number</t>
   </si>
   <si>
-    <t>Technical requirements</t>
-  </si>
-  <si>
     <t>UKPRN</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>UK Provider Reference Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core </t>
-  </si>
-  <si>
     <t xml:space="preserve">2 digits   </t>
   </si>
   <si>
     <t>01</t>
   </si>
   <si>
-    <t>Specialism 1</t>
-  </si>
-  <si>
     <t>3 digits</t>
   </si>
   <si>
     <t xml:space="preserve">         </t>
   </si>
   <si>
-    <t>Specialism 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">8 digits         </t>
   </si>
   <si>
@@ -110,6 +90,9 @@
     <t xml:space="preserve">001 </t>
   </si>
   <si>
+    <t>Format DDMMYYYY</t>
+  </si>
+  <si>
     <t xml:space="preserve">No </t>
   </si>
   <si>
@@ -159,6 +142,21 @@
   </si>
   <si>
     <t>Surveying and Design for Construction and the Built Environment</t>
+  </si>
+  <si>
+    <t>Specialism name</t>
+  </si>
+  <si>
+    <t>Specialism 1 code</t>
+  </si>
+  <si>
+    <t>Specialism 2 code</t>
+  </si>
+  <si>
+    <t>Version 1.0</t>
+  </si>
+  <si>
+    <t>Last updated: 2 May 2020</t>
   </si>
   <si>
     <r>
@@ -181,25 +179,56 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Enter all mandatory data items for a Unique Learner Number (ULN). If this ULN already exists we will overwrite the data we hold with this new data.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+Enter all mandatory data items for a Unique Learner Number (ULN). If this ULN already exists we will overwrite the data we hold with this new data.
 </t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
+    <t>T Levels student registration data: how to use this guide</t>
+  </si>
+  <si>
+    <t>ULN</t>
+  </si>
+  <si>
+    <t>Specialism code 1</t>
+  </si>
+  <si>
+    <t>Specialism code 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can only accept files that:
+* are in CSV format
+* include all mandatory fields
+* contain between one and 10,000 registrations
 </t>
-    </r>
+  </si>
+  <si>
+    <t>UK Register of Learning Providers</t>
+  </si>
+  <si>
+    <t>Learning Records Service - GOV.UK</t>
+  </si>
+  <si>
+    <t>Links to help find data item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This spreadsheet helps awarding organisations to upload registration data to the Manage T Level results service. It contains instructions on how to define the data extract in your own systems and then upload it to an ESFA portal. 
+The tabs have instructions and information on:
+* file data items and format 
+* core and specialism codes
+It also contains an example CSV file. 
+</t>
+  </si>
+  <si>
+    <t>Provider's UK Provider Reference Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course start date </t>
+  </si>
+  <si>
+    <t>Course start date</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -224,60 +253,12 @@
 </t>
     </r>
   </si>
-  <si>
-    <t>Add and edit registrations</t>
-  </si>
-  <si>
-    <t>Specialism name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-We can only accept files that:
-* are in CSV format
-* include all mandatory fields
-* contain a minimum of one or a maximum of 10,000 registrations
-</t>
-  </si>
-  <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>Specialism 1 code</t>
-  </si>
-  <si>
-    <t>Specialism 2 code</t>
-  </si>
-  <si>
-    <t>Version 1.0</t>
-  </si>
-  <si>
-    <t>Last updated: 2 May 2020</t>
-  </si>
-  <si>
-    <t>T Levels student registration data: format and rules guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This spreadsheet helps awarding organisations to upload registration data to the Manage T Level results service. 
-The tabs have instructions and information on:
-* adding and editing registrations
-* technical requirements
-* file data items
-* core and specialism codes
-It also contains an example CSV file. 
-</t>
-  </si>
-  <si>
-    <t>DDMMYYYY</t>
-  </si>
-  <si>
-    <t>ULN</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +279,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -323,10 +312,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -367,8 +357,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,36 +681,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6974FD9F-D6A5-4EB1-B896-7528F68DEE3F}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="48.84375" customWidth="1"/>
+    <col min="1" max="1" width="94.15234375" customWidth="1"/>
+    <col min="2" max="2" width="41.23046875" customWidth="1"/>
+    <col min="3" max="3" width="39.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" ht="160.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:1" ht="174.9" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>52</v>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -719,85 +732,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045182AD-D42E-4E00-B048-4C9A7F723173}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4E3834-5A67-4E3A-8B1D-C1FEB4C54B9D}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="61.921875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="102" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACA1CC8-1D04-47F6-B4D3-AB3426A67E2B}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="52.23046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4E3834-5A67-4E3A-8B1D-C1FEB4C54B9D}">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.3828125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.3828125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.921875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.61328125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="27" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.53515625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.69140625" style="3"/>
+    <col min="3" max="3" width="12.84375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.07421875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.921875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.69140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -813,8 +766,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -830,119 +786,136 @@
       <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="F3" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8">
         <v>10010023</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:B13"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{745A6AA6-48AE-484A-9512-652783CA0F16}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{7EB61F5E-1FEA-4253-A639-FBEE68A8EB62}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <ignoredErrors>
     <ignoredError sqref="C5:C8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41EE773-50EA-462F-B3D6-E499232B5C58}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -961,74 +934,74 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1040,19 +1013,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5F3772-92E8-4979-9794-FD92B6BBE9D3}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.53515625" customWidth="1"/>
-    <col min="2" max="2" width="10.15234375" customWidth="1"/>
-    <col min="3" max="3" width="10.921875" customWidth="1"/>
+    <col min="1" max="1" width="27.4609375" customWidth="1"/>
+    <col min="2" max="2" width="19.07421875" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" customWidth="1"/>
     <col min="4" max="4" width="10.23046875" customWidth="1"/>
     <col min="5" max="5" width="15.921875" customWidth="1"/>
     <col min="6" max="6" width="16.53515625" customWidth="1"/>
@@ -1060,22 +1033,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1089,10 +1062,10 @@
         <v>10102020</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F2" s="10"/>
     </row>
@@ -1107,13 +1080,13 @@
         <v>10102020</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1127,7 +1100,7 @@
         <v>12102020</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>

</xml_diff>

<commit_message>
Updated for Sprint 10
</commit_message>
<xml_diff>
--- a/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
+++ b/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63ef8ac642a543be/MyCo/Clients/SFA/Projects/tl-results-prototype/app/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6D1BBA2-A979-4757-9918-1373E38A0887}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" tabRatio="659" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" tabRatio="659" activeTab="3" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use this guide" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Data item</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>Specialism name</t>
-  </si>
-  <si>
-    <t>Specialism 1 code</t>
-  </si>
-  <si>
-    <t>Specialism 2 code</t>
   </si>
   <si>
     <t>Version 1.0</t>
@@ -252,6 +246,30 @@
 Enter all mandatory data items for an existing ULN. If this ULN already exists we will overwrite the data we hold. If this ULN does not exist we will add it as a new registration.
 </t>
     </r>
+  </si>
+  <si>
+    <t>001, 002</t>
+  </si>
+  <si>
+    <t>Specialism codes</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>01011987</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
   </si>
 </sst>
 </file>
@@ -683,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6974FD9F-D6A5-4EB1-B896-7528F68DEE3F}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -696,34 +714,34 @@
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="1:3" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -787,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -804,15 +822,15 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -843,7 +861,7 @@
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>13</v>
@@ -860,7 +878,7 @@
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>13</v>
@@ -883,7 +901,7 @@
     </row>
     <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="18"/>
       <c r="F13" s="17"/>
@@ -1015,100 +1033,121 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5F3772-92E8-4979-9794-FD92B6BBE9D3}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="27.4609375" customWidth="1"/>
-    <col min="2" max="2" width="19.07421875" customWidth="1"/>
-    <col min="3" max="3" width="17.4609375" customWidth="1"/>
-    <col min="4" max="4" width="10.23046875" customWidth="1"/>
-    <col min="5" max="5" width="15.921875" customWidth="1"/>
-    <col min="6" max="6" width="16.53515625" customWidth="1"/>
+    <col min="2" max="4" width="27.4609375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="19.07421875" customWidth="1"/>
+    <col min="6" max="6" width="17.4609375" customWidth="1"/>
+    <col min="7" max="7" width="10.23046875" customWidth="1"/>
+    <col min="8" max="8" width="15.921875" customWidth="1"/>
+    <col min="9" max="9" width="16.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="12">
         <v>2452343456</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="12">
         <v>12345678</v>
       </c>
-      <c r="C2" s="12">
+      <c r="F2" s="12">
         <v>10102020</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>7646534777</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12">
         <v>87654321</v>
       </c>
-      <c r="C3" s="12">
+      <c r="F3" s="12">
         <v>10102020</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="12">
         <v>9876765555</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12">
         <v>12344321</v>
       </c>
-      <c r="C4" s="12">
+      <c r="F4" s="12">
         <v>12102020</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D4 E2:E3 F3" numberStoredAsText="1"/>
+    <ignoredError sqref="G2:G4 H2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for research today
</commit_message>
<xml_diff>
--- a/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
+++ b/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6D1BBA2-A979-4757-9918-1373E38A0887}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" tabRatio="659" activeTab="3" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="659" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use this guide" sheetId="6" r:id="rId1"/>
@@ -701,45 +701,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6974FD9F-D6A5-4EB1-B896-7528F68DEE3F}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.15234375" customWidth="1"/>
-    <col min="2" max="2" width="41.23046875" customWidth="1"/>
-    <col min="3" max="3" width="39.61328125" customWidth="1"/>
+    <col min="1" max="1" width="94.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:3" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -757,18 +757,18 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.3828125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.921875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.921875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36.07421875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52.921875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.69140625" style="3"/>
+    <col min="1" max="1" width="30.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -808,7 +808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -828,7 +828,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>50</v>
       </c>
@@ -842,7 +842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -859,7 +859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>42</v>
       </c>
@@ -876,7 +876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
@@ -893,28 +893,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="18"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
     </row>
   </sheetData>
@@ -941,16 +941,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.61328125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.23046875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="58.07421875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="55" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.69140625" style="8"/>
+    <col min="5" max="16384" width="8.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -964,7 +964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
@@ -978,7 +978,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -988,7 +988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
@@ -998,7 +998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -1008,7 +1008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1035,22 +1035,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5F3772-92E8-4979-9794-FD92B6BBE9D3}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.4609375" customWidth="1"/>
-    <col min="2" max="4" width="27.4609375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19.07421875" customWidth="1"/>
-    <col min="6" max="6" width="17.4609375" customWidth="1"/>
-    <col min="7" max="7" width="10.23046875" customWidth="1"/>
-    <col min="8" max="8" width="15.921875" customWidth="1"/>
-    <col min="9" max="9" width="16.53515625" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="4" width="27.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>2452343456</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>7646534777</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>9876765555</v>
       </c>

</xml_diff>

<commit_message>
Updated Add and Change journeys
</commit_message>
<xml_diff>
--- a/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
+++ b/app/assets/files/T-Levels-registration-data-format-and-rules-guide-v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63ef8ac642a543be/MyCo/Clients/SFA/Projects/tl-results-prototype/app/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6D1BBA2-A979-4757-9918-1373E38A0887}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{71EED8F8-6447-4AEC-9390-C0163ABDBB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B06A1DF-AB1D-440F-BDAE-E654E983C91E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="659" xr2:uid="{C9AA0910-74FC-48F3-9563-1A22EE5EEB80}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>Data item</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t xml:space="preserve">31092020 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">001 </t>
-  </si>
-  <si>
-    <t>Format DDMMYYYY</t>
   </si>
   <si>
     <t xml:space="preserve">No </t>
@@ -184,12 +178,6 @@
     <t>ULN</t>
   </si>
   <si>
-    <t>Specialism code 1</t>
-  </si>
-  <si>
-    <t>Specialism code 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">We can only accept files that:
 * are in CSV format
 * include all mandatory fields
@@ -221,6 +209,73 @@
   </si>
   <si>
     <t>Course start date</t>
+  </si>
+  <si>
+    <t>001, 002</t>
+  </si>
+  <si>
+    <t>Specialism codes</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>01011987</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Validation rules</t>
+  </si>
+  <si>
+    <t>The whole file will be rejected if one or more errors are found</t>
+  </si>
+  <si>
+    <t>All mandatory fields are required</t>
+  </si>
+  <si>
+    <t>DDMMYYYY</t>
+  </si>
+  <si>
+    <t>Format rules must be followed</t>
+  </si>
+  <si>
+    <t>ULN must not already have an active registration with another Awarding Organisation</t>
+  </si>
+  <si>
+    <t>Core code must be one that is found on the 'Core and specialism codes' tab</t>
+  </si>
+  <si>
+    <t>Specialism code must be one that is found on the 'Core and specialism codes' tab</t>
+  </si>
+  <si>
+    <t>The header row must be added to the CSV file (see Example CSV file' tab</t>
+  </si>
+  <si>
+    <t>Use codes tab below
+Multiple codes must be separated with commas</t>
+  </si>
+  <si>
+    <t>01011990</t>
+  </si>
+  <si>
+    <t>150 chars</t>
+  </si>
+  <si>
+    <t>Date of birth must be in the past</t>
+  </si>
+  <si>
+    <t>UKPRN must exist on the UK Register of Learning Providers</t>
   </si>
   <si>
     <r>
@@ -243,40 +298,16 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Enter all mandatory data items for an existing ULN. If this ULN already exists we will overwrite the data we hold. If this ULN does not exist we will add it as a new registration.
+Enter all mandatory data items for an existing ULN. If this ULN already exists we will overwrite the data we hold. If this ULN does not exist we will add it as a new registration. In regards to specialism codes, if your updated registration contains no specialisms and our records do, then we'll remove the specialism codes from our records.
 </t>
     </r>
-  </si>
-  <si>
-    <t>001, 002</t>
-  </si>
-  <si>
-    <t>Specialism codes</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>01011987</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +337,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,7 +393,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -382,6 +425,37 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -702,7 +776,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,36 +786,36 @@
     <col min="3" max="3" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -751,17 +825,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4E3834-5A67-4E3A-8B1D-C1FEB4C54B9D}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="52.85546875" style="3" customWidth="1"/>
@@ -775,7 +849,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -785,150 +859,248 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>1002345567</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7">
+        <v>10010023</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8">
-        <v>10010023</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B8" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="F13" s="17"/>
+      <c r="E10" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{745A6AA6-48AE-484A-9512-652783CA0F16}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{745A6AA6-48AE-484A-9512-652783CA0F16}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{7EB61F5E-1FEA-4253-A639-FBEE68A8EB62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="C5:C8" numberStoredAsText="1"/>
+    <ignoredError sqref="C8:C9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -943,83 +1115,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="55" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="38.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="55" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1041,8 +1213,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="4" width="27.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15" style="9" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
@@ -1051,98 +1225,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>2452343456</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="D2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="F2" s="11">
+        <v>10102020</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>7646534777</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11">
+        <v>87654321</v>
+      </c>
+      <c r="F3" s="11">
+        <v>10102020</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>9876765555</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11">
+        <v>12344321</v>
+      </c>
+      <c r="F4" s="11">
+        <v>12102020</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>2452343456</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="12">
-        <v>12345678</v>
-      </c>
-      <c r="F2" s="12">
-        <v>10102020</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>7646534777</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12">
-        <v>87654321</v>
-      </c>
-      <c r="F3" s="12">
-        <v>10102020</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>9876765555</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12">
-        <v>12344321</v>
-      </c>
-      <c r="F4" s="12">
-        <v>12102020</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>